<commit_message>
tamoc-119: use hash index (#5033)
</commit_message>
<xml_diff>
--- a/packages/sync-server/exported-refdata-all-table.xlsx
+++ b/packages/sync-server/exported-refdata-all-table.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,45 +415,51 @@
         <v>email</v>
       </c>
       <c r="K1" t="str">
+        <v>visibilityStatus</v>
+      </c>
+      <c r="L1" t="str">
         <v>villageId</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>mergedIntoId</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>3cf6cc61-e682-41ba-aa96-7a46ebef428e</v>
+        <v>7e34e48c-6482-4e81-9fea-de3a04724635</v>
       </c>
       <c r="B2" t="str">
-        <v>NKIX135928</v>
+        <v>UTLE519661</v>
       </c>
       <c r="C2" t="str">
-        <v>Helena</v>
+        <v>Betty</v>
       </c>
       <c r="E2" t="str">
-        <v>Gabbrielli</v>
+        <v>Thompson</v>
       </c>
       <c r="F2" t="str">
-        <v>Inoue</v>
+        <v>Louis</v>
       </c>
       <c r="G2" s="1">
-        <v>38106.5</v>
+        <v>33574</v>
       </c>
       <c r="I2" t="str">
         <v>female</v>
       </c>
+      <c r="K2" t="str">
+        <v>current</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -468,6 +474,9 @@
       <c r="C1" t="str">
         <v>name</v>
       </c>
+      <c r="D1" t="str">
+        <v>visibilityStatus</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -479,6 +488,9 @@
       <c r="C2" t="str">
         <v>Sesame</v>
       </c>
+      <c r="D2" t="str">
+        <v>current</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -490,17 +502,20 @@
       <c r="C3" t="str">
         <v>Wheat</v>
       </c>
+      <c r="D3" t="str">
+        <v>current</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -515,6 +530,9 @@
       <c r="C1" t="str">
         <v>name</v>
       </c>
+      <c r="D1" t="str">
+        <v>visibilityStatus</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -526,6 +544,9 @@
       <c r="C2" t="str">
         <v>Myofibrosis</v>
       </c>
+      <c r="D2" t="str">
+        <v>current</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -537,10 +558,13 @@
       <c r="C3" t="str">
         <v>Thigh injury</v>
       </c>
+      <c r="D3" t="str">
+        <v>current</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "tamoc-119: use hash index (#5033)"
This reverts commit 8320412dbde96cc92e5d0d98451949accb0600c8.
</commit_message>
<xml_diff>
--- a/packages/sync-server/exported-refdata-all-table.xlsx
+++ b/packages/sync-server/exported-refdata-all-table.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,51 +415,45 @@
         <v>email</v>
       </c>
       <c r="K1" t="str">
-        <v>visibilityStatus</v>
+        <v>villageId</v>
       </c>
       <c r="L1" t="str">
-        <v>villageId</v>
-      </c>
-      <c r="M1" t="str">
         <v>mergedIntoId</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>7e34e48c-6482-4e81-9fea-de3a04724635</v>
+        <v>3cf6cc61-e682-41ba-aa96-7a46ebef428e</v>
       </c>
       <c r="B2" t="str">
-        <v>UTLE519661</v>
+        <v>NKIX135928</v>
       </c>
       <c r="C2" t="str">
-        <v>Betty</v>
+        <v>Helena</v>
       </c>
       <c r="E2" t="str">
-        <v>Thompson</v>
+        <v>Gabbrielli</v>
       </c>
       <c r="F2" t="str">
-        <v>Louis</v>
+        <v>Inoue</v>
       </c>
       <c r="G2" s="1">
-        <v>33574</v>
+        <v>38106.5</v>
       </c>
       <c r="I2" t="str">
         <v>female</v>
       </c>
-      <c r="K2" t="str">
-        <v>current</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -474,9 +468,6 @@
       <c r="C1" t="str">
         <v>name</v>
       </c>
-      <c r="D1" t="str">
-        <v>visibilityStatus</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -488,9 +479,6 @@
       <c r="C2" t="str">
         <v>Sesame</v>
       </c>
-      <c r="D2" t="str">
-        <v>current</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -502,20 +490,17 @@
       <c r="C3" t="str">
         <v>Wheat</v>
       </c>
-      <c r="D3" t="str">
-        <v>current</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -530,9 +515,6 @@
       <c r="C1" t="str">
         <v>name</v>
       </c>
-      <c r="D1" t="str">
-        <v>visibilityStatus</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -544,9 +526,6 @@
       <c r="C2" t="str">
         <v>Myofibrosis</v>
       </c>
-      <c r="D2" t="str">
-        <v>current</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -558,13 +537,10 @@
       <c r="C3" t="str">
         <v>Thigh injury</v>
       </c>
-      <c r="D3" t="str">
-        <v>current</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "tamoc-119: use hash index (#5033)" (#5067)
This reverts commit 8320412dbde96cc92e5d0d98451949accb0600c8.
</commit_message>
<xml_diff>
--- a/packages/sync-server/exported-refdata-all-table.xlsx
+++ b/packages/sync-server/exported-refdata-all-table.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,51 +415,45 @@
         <v>email</v>
       </c>
       <c r="K1" t="str">
-        <v>visibilityStatus</v>
+        <v>villageId</v>
       </c>
       <c r="L1" t="str">
-        <v>villageId</v>
-      </c>
-      <c r="M1" t="str">
         <v>mergedIntoId</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>7e34e48c-6482-4e81-9fea-de3a04724635</v>
+        <v>3cf6cc61-e682-41ba-aa96-7a46ebef428e</v>
       </c>
       <c r="B2" t="str">
-        <v>UTLE519661</v>
+        <v>NKIX135928</v>
       </c>
       <c r="C2" t="str">
-        <v>Betty</v>
+        <v>Helena</v>
       </c>
       <c r="E2" t="str">
-        <v>Thompson</v>
+        <v>Gabbrielli</v>
       </c>
       <c r="F2" t="str">
-        <v>Louis</v>
+        <v>Inoue</v>
       </c>
       <c r="G2" s="1">
-        <v>33574</v>
+        <v>38106.5</v>
       </c>
       <c r="I2" t="str">
         <v>female</v>
       </c>
-      <c r="K2" t="str">
-        <v>current</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -474,9 +468,6 @@
       <c r="C1" t="str">
         <v>name</v>
       </c>
-      <c r="D1" t="str">
-        <v>visibilityStatus</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -488,9 +479,6 @@
       <c r="C2" t="str">
         <v>Sesame</v>
       </c>
-      <c r="D2" t="str">
-        <v>current</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -502,20 +490,17 @@
       <c r="C3" t="str">
         <v>Wheat</v>
       </c>
-      <c r="D3" t="str">
-        <v>current</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -530,9 +515,6 @@
       <c r="C1" t="str">
         <v>name</v>
       </c>
-      <c r="D1" t="str">
-        <v>visibilityStatus</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -544,9 +526,6 @@
       <c r="C2" t="str">
         <v>Myofibrosis</v>
       </c>
-      <c r="D2" t="str">
-        <v>current</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -558,13 +537,10 @@
       <c r="C3" t="str">
         <v>Thigh injury</v>
       </c>
-      <c r="D3" t="str">
-        <v>current</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>